<commit_message>
Small update to README
</commit_message>
<xml_diff>
--- a/Provider_Market_Data.xlsx
+++ b/Provider_Market_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Projects/CCAF/crypto-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC0402-8B46-B243-B777-43CC071F78D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF855C-08B5-9944-9CC0-FD9020AFE0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26220" yWindow="3140" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1700" windowWidth="36300" windowHeight="23240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,11 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -802,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -831,7 +830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -860,7 +859,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -886,7 +885,7 @@
         <v>0.99567154474995045</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -915,7 +914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -944,7 +943,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -970,7 +969,7 @@
         <v>0.99984606379865004</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -999,7 +998,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>0.99969537829285593</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1225,7 +1224,7 @@
         <v>0.98307555454121864</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1254,7 +1253,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1338,7 +1337,7 @@
         <v>1.003056162993756</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>4.5975889285052007</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1506,7 +1505,7 @@
         <v>0.99958582307203003</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>0.86355227359962405</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>0.99754781241261703</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1842,7 +1841,7 @@
         <v>1.016</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>2.14857460171062</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>1.70117112316715</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>1.004765866737795</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2036,7 +2035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>2.131591E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>0.999403997369959</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -2175,7 +2174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>0.99937843347638478</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>0.99853198120585895</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -2314,7 +2313,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>0.99913376452892455</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>46</v>
       </c>
@@ -2424,7 +2423,7 @@
         <v>0.99986010987726504</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2481,11 +2480,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J66" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Binance USD"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J66">
       <sortCondition ref="C1:C66"/>
     </sortState>

</xml_diff>